<commit_message>
inetbanking updated adding new customer
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetBanking/TestData/LoginData.xlsx
+++ b/src/test/java/com/inetBanking/TestData/LoginData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="14350" windowHeight="5300"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -30,16 +31,10 @@
     <t>jUsugar</t>
   </si>
   <si>
-    <t>mngr164225</t>
-  </si>
-  <si>
-    <t>jahetAp</t>
-  </si>
-  <si>
-    <t>mngr1111</t>
-  </si>
-  <si>
-    <t>jttttt</t>
+    <t>mngr523220</t>
+  </si>
+  <si>
+    <t>gynUnYd</t>
   </si>
 </sst>
 </file>
@@ -392,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -420,7 +415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -428,14 +423,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>